<commit_message>
feat: :sparkles: Tools and Excel features implemented
</commit_message>
<xml_diff>
--- a/data/example.xlsx
+++ b/data/example.xlsx
@@ -399,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -418,10 +418,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>alice@example.com</v>
+        <v>test777@email.com</v>
       </c>
       <c r="B2" t="str">
-        <v>Alice</v>
+        <v>Test Value 1768868373503</v>
       </c>
       <c r="C2">
         <v>90</v>

</xml_diff>